<commit_message>
matrice e WBS incrociate
</commit_message>
<xml_diff>
--- a/Documenti/Pianificazione/matrice delle responsabilità.xlsx
+++ b/Documenti/Pianificazione/matrice delle responsabilità.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
   <si>
     <t>Project Manager</t>
   </si>
@@ -621,7 +621,7 @@
   <dimension ref="B2:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -780,9 +780,13 @@
       <c r="B10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>

</xml_diff>